<commit_message>
update file directory and name
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_dataset_directoryFilename.xlsx
+++ b/Load/ontology/harmonization/clinEpi_dataset_directoryFilename.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A29609-F18F-A84E-879B-E7B2EAC69DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C56DBBD-F47D-E943-A7F9-15691F50F164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="28040" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="460" windowWidth="28040" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clinEpi_dataset_directoryFilena" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="303">
   <si>
     <t>Project category directory</t>
   </si>
@@ -635,13 +635,307 @@
   </si>
   <si>
     <t>WestAfrica_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>washb_bangladesh</t>
+  </si>
+  <si>
+    <t>gates_washb_bangladesh.owl</t>
+  </si>
+  <si>
+    <t>gates_score_rwanda.owl</t>
+  </si>
+  <si>
+    <t>gates_score_burundi.owl</t>
+  </si>
+  <si>
+    <t>score_sm_crt</t>
+  </si>
+  <si>
+    <t>gates_score_sm_crt.owl</t>
+  </si>
+  <si>
+    <t>GEMS1A_HUAS</t>
+  </si>
+  <si>
+    <t>gates_maled.owl</t>
+  </si>
+  <si>
+    <t>washb_kenya</t>
+  </si>
+  <si>
+    <t>gates_washb_kenya.owl</t>
+  </si>
+  <si>
+    <t>SCORE_Five_Country</t>
+  </si>
+  <si>
+    <t>gates_score_five_country.owl</t>
+  </si>
+  <si>
+    <t>gates_score_moz.owl</t>
+  </si>
+  <si>
+    <t>ganc</t>
+  </si>
+  <si>
+    <t>gates_score_seasonal.owl</t>
+  </si>
+  <si>
+    <t>GEMS_HUAS</t>
+  </si>
+  <si>
+    <t>gates_score_nig.owl</t>
+  </si>
+  <si>
+    <t>gates_score_zanzibar.owl</t>
+  </si>
+  <si>
+    <t>SCORE_sm_cohort</t>
+  </si>
+  <si>
+    <t>gates_score_sm_cohort.owl</t>
+  </si>
+  <si>
+    <t>icemr_south_asia.owl</t>
+  </si>
+  <si>
+    <t>icemr_southern_africa.owl</t>
+  </si>
+  <si>
+    <t>india_cohort</t>
+  </si>
+  <si>
+    <t>icemr_india_cohort.owl</t>
+  </si>
+  <si>
+    <t>icemr_india_meghalaya.owl</t>
+  </si>
+  <si>
+    <t>india_severe_malaria</t>
+  </si>
+  <si>
+    <t>icemr_india_severe_malaria.owl</t>
+  </si>
+  <si>
+    <t>amazonia_Peru</t>
+  </si>
+  <si>
+    <t>icemr_amazonia_peru.owl</t>
+  </si>
+  <si>
+    <t>icemr_west_africa.owl</t>
+  </si>
+  <si>
+    <t>amazonia_Brazil</t>
+  </si>
+  <si>
+    <t>icemr_amazonia_brazil.owl</t>
+  </si>
+  <si>
+    <t>india_fever_surv</t>
+  </si>
+  <si>
+    <t>icemr_india_fever_surv.owl</t>
+  </si>
+  <si>
+    <t>india_cx</t>
+  </si>
+  <si>
+    <t>icemr_india_cx.owl</t>
+  </si>
+  <si>
+    <t>icemr_southeast_asia.owl</t>
+  </si>
+  <si>
+    <t>general_promote.owl</t>
+  </si>
+  <si>
+    <t>covid19_india</t>
+  </si>
+  <si>
+    <t>general_covid19_india.owl</t>
+  </si>
+  <si>
+    <t>kalifabougou</t>
+  </si>
+  <si>
+    <t>general_kalifabougou.owl</t>
+  </si>
+  <si>
+    <t>Updated directory and file names</t>
+  </si>
+  <si>
+    <t>score_sm_crt_conversion.csv</t>
+  </si>
+  <si>
+    <t>gems1a_huas_conversion.csv</t>
+  </si>
+  <si>
+    <t>MALED_conversion.csv</t>
+  </si>
+  <si>
+    <t>WASHb_Kenya_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_five_country_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_moz_conversion.csv</t>
+  </si>
+  <si>
+    <t>ganc_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_seasonal_conversion.csv</t>
+  </si>
+  <si>
+    <t>gems_huas_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_nig_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_zanzibar_conversion.csv</t>
+  </si>
+  <si>
+    <t>promote_conversion.csv</t>
+  </si>
+  <si>
+    <t>covid19_india_conversion.csv</t>
+  </si>
+  <si>
+    <t>hcq_non_randomized_conversion.csv</t>
+  </si>
+  <si>
+    <t>kalifabougou_conversion.csv</t>
+  </si>
+  <si>
+    <t>south_asia_conversion.csv</t>
+  </si>
+  <si>
+    <t>southern_africa_conversion.csv</t>
+  </si>
+  <si>
+    <t>malawi_conversion.csv</t>
+  </si>
+  <si>
+    <t>India_cohort_conversion.csv</t>
+  </si>
+  <si>
+    <t>india_meghalaya_conversion.csv</t>
+  </si>
+  <si>
+    <t>india_severe_malaria_conversion.csv</t>
+  </si>
+  <si>
+    <t>amazonia_peru_conversion.csv</t>
+  </si>
+  <si>
+    <t>west_africa_conversion.csv</t>
+  </si>
+  <si>
+    <t>amazonia_brazil_conversion.csv</t>
+  </si>
+  <si>
+    <t>india_fever_surv_conversion.csv</t>
+  </si>
+  <si>
+    <t>India_cx_conversion.csv</t>
+  </si>
+  <si>
+    <t>prism2_border_cohort_conversion.csv</t>
+  </si>
+  <si>
+    <t>southeast_asia_conversion.csv</t>
+  </si>
+  <si>
+    <t>score_sm_crt_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>gems1a_huas_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>WASHb_Kenya_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>score_five_country_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>score_moz_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>ganc_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>score_seasonal_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>gems_huas_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>score_nig_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>score_zanzibar_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>promote_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>covid19_india_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>hcq_non_randomized_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>kalifabougou_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>south_asia_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>southern_africa_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>malawi_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>india_cohort_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>india_meghalaya_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>india_severe_malaria_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>amazonia_peru_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>west_africa_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>amazonia_brazil_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>india_fever_surv_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>India_cx_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>prism2_border_cohort_conversion_temp.csv</t>
+  </si>
+  <si>
+    <t>southeast_asia_conversion_temp.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -772,6 +1066,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1118,9 +1419,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1476,20 +1778,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="43.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
@@ -2506,7 +2808,1033 @@
         <v>204</v>
       </c>
     </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="1" customFormat="1">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>254</v>
+      </c>
+      <c r="F61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>256</v>
+      </c>
+      <c r="F63" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>249</v>
+      </c>
+      <c r="F65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" t="s">
+        <v>208</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71" t="s">
+        <v>216</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>252</v>
+      </c>
+      <c r="F71" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>253</v>
+      </c>
+      <c r="F72" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>257</v>
+      </c>
+      <c r="F73" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" t="s">
+        <v>207</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>70</v>
+      </c>
+      <c r="F74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>255</v>
+      </c>
+      <c r="F75" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>78</v>
+      </c>
+      <c r="F76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>209</v>
+      </c>
+      <c r="C77" t="s">
+        <v>210</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>248</v>
+      </c>
+      <c r="F77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" t="s">
+        <v>222</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>258</v>
+      </c>
+      <c r="F78" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>90</v>
+      </c>
+      <c r="F79" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" t="s">
+        <v>93</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>106</v>
+      </c>
+      <c r="F81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>98</v>
+      </c>
+      <c r="F82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83" t="s">
+        <v>101</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>102</v>
+      </c>
+      <c r="F83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>205</v>
+      </c>
+      <c r="C84" t="s">
+        <v>206</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>213</v>
+      </c>
+      <c r="C85" t="s">
+        <v>214</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>251</v>
+      </c>
+      <c r="F85" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" t="s">
+        <v>117</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>118</v>
+      </c>
+      <c r="F86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" t="s">
+        <v>244</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>260</v>
+      </c>
+      <c r="F87" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" t="s">
+        <v>129</v>
+      </c>
+      <c r="C88" t="s">
+        <v>130</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s">
+        <v>261</v>
+      </c>
+      <c r="F88" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="s">
+        <v>262</v>
+      </c>
+      <c r="F89" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" t="s">
+        <v>134</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s">
+        <v>135</v>
+      </c>
+      <c r="F90" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" t="s">
+        <v>242</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s">
+        <v>259</v>
+      </c>
+      <c r="F91" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" t="s">
+        <v>138</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="s">
+        <v>139</v>
+      </c>
+      <c r="F92" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>144</v>
+      </c>
+      <c r="B93" t="s">
+        <v>235</v>
+      </c>
+      <c r="C93" t="s">
+        <v>236</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
+        <v>271</v>
+      </c>
+      <c r="F93" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>144</v>
+      </c>
+      <c r="B94" t="s">
+        <v>232</v>
+      </c>
+      <c r="C94" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>269</v>
+      </c>
+      <c r="F94" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" t="s">
+        <v>152</v>
+      </c>
+      <c r="C95" t="s">
+        <v>153</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>154</v>
+      </c>
+      <c r="F95" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" t="s">
+        <v>228</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>266</v>
+      </c>
+      <c r="F96" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" t="s">
+        <v>239</v>
+      </c>
+      <c r="C97" t="s">
+        <v>240</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" t="s">
+        <v>273</v>
+      </c>
+      <c r="F97" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" t="s">
+        <v>144</v>
+      </c>
+      <c r="B98" t="s">
+        <v>237</v>
+      </c>
+      <c r="C98" t="s">
+        <v>238</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" t="s">
+        <v>272</v>
+      </c>
+      <c r="F98" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" t="s">
+        <v>229</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" t="s">
+        <v>267</v>
+      </c>
+      <c r="F99" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" t="s">
+        <v>144</v>
+      </c>
+      <c r="B100" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" t="s">
+        <v>231</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>268</v>
+      </c>
+      <c r="F100" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101" t="s">
+        <v>172</v>
+      </c>
+      <c r="C101" t="s">
+        <v>173</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" t="s">
+        <v>265</v>
+      </c>
+      <c r="F101" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" t="s">
+        <v>144</v>
+      </c>
+      <c r="B102" t="s">
+        <v>176</v>
+      </c>
+      <c r="C102" t="s">
+        <v>177</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="s">
+        <v>178</v>
+      </c>
+      <c r="F102" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" t="s">
+        <v>144</v>
+      </c>
+      <c r="B103" t="s">
+        <v>185</v>
+      </c>
+      <c r="C103" t="s">
+        <v>186</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" t="s">
+        <v>144</v>
+      </c>
+      <c r="B104" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" t="s">
+        <v>181</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" t="s">
+        <v>274</v>
+      </c>
+      <c r="F104" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" t="s">
+        <v>144</v>
+      </c>
+      <c r="B105" t="s">
+        <v>189</v>
+      </c>
+      <c r="C105" t="s">
+        <v>225</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" t="s">
+        <v>263</v>
+      </c>
+      <c r="F105" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" t="s">
+        <v>144</v>
+      </c>
+      <c r="B106" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" t="s">
+        <v>241</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" t="s">
+        <v>275</v>
+      </c>
+      <c r="F106" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B107" t="s">
+        <v>197</v>
+      </c>
+      <c r="C107" t="s">
+        <v>226</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" t="s">
+        <v>264</v>
+      </c>
+      <c r="F107" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" t="s">
+        <v>144</v>
+      </c>
+      <c r="B108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
+        <v>234</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s">
+        <v>270</v>
+      </c>
+      <c r="F108" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H59:K112">
+    <sortCondition ref="H59:H112"/>
+    <sortCondition ref="I59:I112"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>